<commit_message>
Adicionando o botão de gerar crachá
</commit_message>
<xml_diff>
--- a/CRACHA DE SEGURANÇA - CONCREJATO MODELO.xlsx
+++ b/CRACHA DE SEGURANÇA - CONCREJATO MODELO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a1ebf6dd240dbab/Documentos/Programas.py/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a1ebf6dd240dbab/Documentos/RPA-cjato/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="8_{DB59C3B0-4429-4B58-95CC-A54F743C3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF549704-94F5-452A-91D9-A8170058AE9B}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="8_{DB59C3B0-4429-4B58-95CC-A54F743C3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA4D0BD-E9BB-437B-A4A9-F06C006CF40C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D084067-D632-477E-9D38-2AE12336750E}"/>
   </bookViews>
@@ -2350,13 +2350,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="850" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>GILMAR INACIO DE OLIVEIRA</a:t>
-          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="850" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2417,13 +2414,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="850">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>ARMADOR</a:t>
-          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="850">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2484,13 +2478,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="850" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>28/01/2026</a:t>
-          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="850" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2551,13 +2542,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="850">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>MCA CONSTRUÇÕES E REFORMAS</a:t>
-          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="850">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3954,7 +3942,7 @@
   <dimension ref="B1:BO22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N11"/>
+      <selection activeCell="BC15" sqref="BC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4694,23 +4682,15 @@
       <c r="BO11" s="14"/>
     </row>
     <row r="12" spans="2:67" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15">
-        <v>45686</v>
-      </c>
-      <c r="C12" s="16">
-        <v>45687</v>
-      </c>
-      <c r="D12" s="18">
-        <v>45686</v>
-      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="18">
-        <v>45688</v>
-      </c>
+      <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
@@ -4771,14 +4751,14 @@
       <c r="BO12" s="14"/>
     </row>
     <row r="13" spans="2:67" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="56">
+      <c r="B13" s="56" t="str">
         <f>IF(B12,B12+730," ")</f>
-        <v>46416</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C13" s="57"/>
-      <c r="D13" s="48">
+      <c r="D13" s="48" t="str">
         <f>IF(D12,D12+730," ")</f>
-        <v>46416</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E13" s="48" t="str">
         <f>IF(E12,E12+1826," ")</f>
@@ -4800,9 +4780,9 @@
         <f>IF(I12,I12+365," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J13" s="48">
+      <c r="J13" s="48" t="str">
         <f>IF(J12,J12+1095," ")</f>
-        <v>46783</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="K13" s="48" t="str">
         <f>IF(K12,K12+1095," ")</f>
@@ -5361,6 +5341,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C71207AC7C1B264DB9730F1A1A91D442" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="b60db062c4fb830cf3a1b9a88bd9eca0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45d94a95-bf6f-476b-a44a-2dd9d8893bc6" xmlns:ns3="b5929ff3-2a6a-438e-8c42-a595e58ba94d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aecf9f73066d20b296ec6999cae6960" ns2:_="" ns3:_="">
     <xsd:import namespace="45d94a95-bf6f-476b-a44a-2dd9d8893bc6"/>
@@ -5573,7 +5562,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b5929ff3-2a6a-438e-8c42-a595e58ba94d"/>
@@ -5584,16 +5573,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B29A280-6F30-48D7-8F10-95835ABF11CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC58EBBC-891A-4294-A25F-34B3130C148C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5612,7 +5600,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D74C3698-C988-4341-A94D-C16ABA905960}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5621,12 +5609,4 @@
     <ds:schemaRef ds:uri="45d94a95-bf6f-476b-a44a-2dd9d8893bc6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B29A280-6F30-48D7-8F10-95835ABF11CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrigindo fórmula no xlsx
</commit_message>
<xml_diff>
--- a/CRACHA DE SEGURANÇA - CONCREJATO MODELO.xlsx
+++ b/CRACHA DE SEGURANÇA - CONCREJATO MODELO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a1ebf6dd240dbab/Documentos/RPA-cjato/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="8_{DB59C3B0-4429-4B58-95CC-A54F743C3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA4D0BD-E9BB-437B-A4A9-F06C006CF40C}"/>
+  <xr:revisionPtr revIDLastSave="391" documentId="8_{DB59C3B0-4429-4B58-95CC-A54F743C3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EEFA785-D810-429C-9401-BEA0B53CEABE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D084067-D632-477E-9D38-2AE12336750E}"/>
   </bookViews>
@@ -3942,7 +3942,7 @@
   <dimension ref="B1:BO22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="BC15" sqref="BC15"/>
+      <selection activeCell="C13" sqref="C13:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4755,7 +4755,10 @@
         <f>IF(B12,B12+730," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="57" t="str">
+        <f>IF(C12,C12+730," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="D13" s="48" t="str">
         <f>IF(D12,D12+730," ")</f>
         <v xml:space="preserve"> </v>
@@ -5326,12 +5329,9 @@
     <mergeCell ref="G3:G11"/>
     <mergeCell ref="C3:C11"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH20" xr:uid="{103330E7-9B97-472D-AA6C-9D1CA200D122}">
       <formula1>$BK$8:$BK$14</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B19 D17:N19 C17 C19" xr:uid="{E7312F84-69D5-4BCC-A0AB-B88C0F3844A3}">
-      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>